<commit_message>
updated xml and xlsx.
</commit_message>
<xml_diff>
--- a/DividendLiberty/Dividend Calculation.xlsx
+++ b/DividendLiberty/Dividend Calculation.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12795" windowHeight="11985" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12792" windowHeight="11988"/>
   </bookViews>
   <sheets>
     <sheet name="Yearly" sheetId="1" r:id="rId1"/>
     <sheet name="All Time" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -96,7 +96,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -358,6 +358,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -393,6 +410,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -547,26 +581,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="1">
         <v>2016</v>
       </c>
     </row>
-    <row r="2" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:7" ht="18" x14ac:dyDescent="0.35">
       <c r="C2" s="7" t="s">
         <v>0</v>
       </c>
@@ -583,7 +617,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:7" ht="18" x14ac:dyDescent="0.35">
       <c r="B3" s="7">
         <v>1</v>
       </c>
@@ -604,7 +638,7 @@
         <v>30.66</v>
       </c>
     </row>
-    <row r="4" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:7" ht="18" x14ac:dyDescent="0.35">
       <c r="B4" s="7">
         <v>2</v>
       </c>
@@ -625,7 +659,7 @@
         <v>73.209999999999994</v>
       </c>
     </row>
-    <row r="5" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:7" ht="18" x14ac:dyDescent="0.35">
       <c r="B5" s="7">
         <v>3</v>
       </c>
@@ -646,7 +680,7 @@
         <v>117.92</v>
       </c>
     </row>
-    <row r="6" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:7" ht="18" x14ac:dyDescent="0.35">
       <c r="B6" s="7">
         <v>4</v>
       </c>
@@ -667,7 +701,7 @@
         <v>37.21</v>
       </c>
     </row>
-    <row r="7" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:7" ht="18" x14ac:dyDescent="0.35">
       <c r="B7" s="7">
         <v>5</v>
       </c>
@@ -688,7 +722,7 @@
         <v>70.34</v>
       </c>
     </row>
-    <row r="8" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:7" ht="18" x14ac:dyDescent="0.35">
       <c r="B8" s="7">
         <v>6</v>
       </c>
@@ -709,7 +743,7 @@
         <v>145.80000000000001</v>
       </c>
     </row>
-    <row r="9" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:7" ht="18" x14ac:dyDescent="0.35">
       <c r="B9" s="7">
         <v>7</v>
       </c>
@@ -730,7 +764,7 @@
         <v>22.35</v>
       </c>
     </row>
-    <row r="10" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:7" ht="18" x14ac:dyDescent="0.35">
       <c r="B10" s="7">
         <v>8</v>
       </c>
@@ -751,7 +785,7 @@
         <v>78.61</v>
       </c>
     </row>
-    <row r="11" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:7" ht="18" x14ac:dyDescent="0.35">
       <c r="B11" s="7">
         <v>9</v>
       </c>
@@ -759,7 +793,7 @@
         <v>13</v>
       </c>
       <c r="D11" s="9">
-        <v>91.54</v>
+        <v>94.57</v>
       </c>
       <c r="E11" s="10">
         <v>31.32</v>
@@ -769,10 +803,10 @@
       </c>
       <c r="G11" s="12">
         <f t="shared" si="0"/>
-        <v>165.85000000000002</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
+        <v>168.88</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="18" x14ac:dyDescent="0.35">
       <c r="B12" s="7">
         <v>10</v>
       </c>
@@ -780,7 +814,7 @@
         <v>14</v>
       </c>
       <c r="D12" s="9">
-        <v>0</v>
+        <v>17.55</v>
       </c>
       <c r="E12" s="10">
         <v>0</v>
@@ -790,10 +824,10 @@
       </c>
       <c r="G12" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
+        <v>17.55</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" ht="18" x14ac:dyDescent="0.35">
       <c r="B13" s="7">
         <v>11</v>
       </c>
@@ -814,7 +848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:7" ht="18" x14ac:dyDescent="0.35">
       <c r="B14" s="7">
         <v>12</v>
       </c>
@@ -834,13 +868,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:7" ht="18" x14ac:dyDescent="0.35">
       <c r="C15" s="14" t="s">
         <v>20</v>
       </c>
       <c r="D15" s="3">
         <f>SUM(D3:D14)</f>
-        <v>569.87</v>
+        <v>590.44999999999993</v>
       </c>
       <c r="E15" s="4">
         <f>SUM(E3:E14)</f>
@@ -852,7 +886,7 @@
       </c>
       <c r="G15" s="6">
         <f>SUM(G3:G14)</f>
-        <v>741.95</v>
+        <v>762.53</v>
       </c>
     </row>
   </sheetData>
@@ -865,27 +899,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="K42" sqref="K42"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="E5" s="17" t="s">
         <v>17</v>
       </c>
@@ -902,7 +936,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="D6" s="7">
         <v>1</v>
       </c>
@@ -923,7 +957,7 @@
         <v>214.47</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="D7" s="7">
         <v>2</v>
       </c>
@@ -931,7 +965,7 @@
         <v>2016</v>
       </c>
       <c r="F7" s="9">
-        <v>569.87</v>
+        <v>590.45000000000005</v>
       </c>
       <c r="G7" s="10">
         <v>42.16</v>
@@ -941,10 +975,10 @@
       </c>
       <c r="I7" s="12">
         <f t="shared" ref="I7:I45" si="0">SUM(F7:H7)</f>
-        <v>741.94999999999993</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+        <v>762.53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="D8" s="7">
         <v>3</v>
       </c>
@@ -965,7 +999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="D9" s="7">
         <v>4</v>
       </c>
@@ -986,7 +1020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="D10" s="7">
         <v>5</v>
       </c>
@@ -1007,7 +1041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="D11" s="7">
         <v>6</v>
       </c>
@@ -1028,7 +1062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="D12" s="7">
         <v>7</v>
       </c>
@@ -1049,7 +1083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="D13" s="7">
         <v>8</v>
       </c>
@@ -1070,7 +1104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="D14" s="7">
         <v>9</v>
       </c>
@@ -1091,7 +1125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="D15" s="7">
         <v>10</v>
       </c>
@@ -1112,7 +1146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="D16" s="7">
         <v>11</v>
       </c>
@@ -1133,7 +1167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="4:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:9" ht="18" x14ac:dyDescent="0.35">
       <c r="D17" s="7">
         <v>12</v>
       </c>
@@ -1154,7 +1188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="4:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="18" spans="4:9" ht="18" x14ac:dyDescent="0.35">
       <c r="D18" s="7">
         <v>13</v>
       </c>
@@ -1175,7 +1209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="4:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="19" spans="4:9" ht="18" x14ac:dyDescent="0.35">
       <c r="D19" s="7">
         <v>14</v>
       </c>
@@ -1196,7 +1230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="4:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="20" spans="4:9" ht="18" x14ac:dyDescent="0.35">
       <c r="D20" s="7">
         <v>15</v>
       </c>
@@ -1217,7 +1251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="4:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="21" spans="4:9" ht="18" x14ac:dyDescent="0.35">
       <c r="D21" s="7">
         <v>16</v>
       </c>
@@ -1238,7 +1272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="4:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="22" spans="4:9" ht="18" x14ac:dyDescent="0.35">
       <c r="D22" s="7">
         <v>17</v>
       </c>
@@ -1259,7 +1293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="4:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="23" spans="4:9" ht="18" x14ac:dyDescent="0.35">
       <c r="D23" s="7">
         <v>18</v>
       </c>
@@ -1280,7 +1314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="4:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="24" spans="4:9" ht="18" x14ac:dyDescent="0.35">
       <c r="D24" s="7">
         <v>19</v>
       </c>
@@ -1301,7 +1335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="4:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="25" spans="4:9" ht="18" x14ac:dyDescent="0.35">
       <c r="D25" s="7">
         <v>20</v>
       </c>
@@ -1322,7 +1356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="4:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="26" spans="4:9" ht="18" x14ac:dyDescent="0.35">
       <c r="D26" s="7">
         <v>21</v>
       </c>
@@ -1343,7 +1377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="4:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="27" spans="4:9" ht="18" x14ac:dyDescent="0.35">
       <c r="D27" s="7">
         <v>22</v>
       </c>
@@ -1364,7 +1398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="4:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="28" spans="4:9" ht="18" x14ac:dyDescent="0.35">
       <c r="D28" s="7">
         <v>23</v>
       </c>
@@ -1385,7 +1419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="4:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="29" spans="4:9" ht="18" x14ac:dyDescent="0.35">
       <c r="D29" s="7">
         <v>24</v>
       </c>
@@ -1406,7 +1440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="4:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="30" spans="4:9" ht="18" x14ac:dyDescent="0.35">
       <c r="D30" s="7">
         <v>25</v>
       </c>
@@ -1427,7 +1461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="4:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="31" spans="4:9" ht="18" x14ac:dyDescent="0.35">
       <c r="D31" s="7">
         <v>26</v>
       </c>
@@ -1448,7 +1482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="4:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="32" spans="4:9" ht="18" x14ac:dyDescent="0.35">
       <c r="D32" s="7">
         <v>27</v>
       </c>
@@ -1469,7 +1503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="4:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="33" spans="4:9" ht="18" x14ac:dyDescent="0.35">
       <c r="D33" s="7">
         <v>28</v>
       </c>
@@ -1490,7 +1524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="4:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="34" spans="4:9" ht="18" x14ac:dyDescent="0.35">
       <c r="D34" s="7">
         <v>29</v>
       </c>
@@ -1511,7 +1545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="4:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="35" spans="4:9" ht="18" x14ac:dyDescent="0.35">
       <c r="D35" s="7">
         <v>30</v>
       </c>
@@ -1532,7 +1566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="4:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="36" spans="4:9" ht="18" x14ac:dyDescent="0.35">
       <c r="D36" s="7">
         <v>31</v>
       </c>
@@ -1553,7 +1587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="4:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="37" spans="4:9" ht="18" x14ac:dyDescent="0.35">
       <c r="D37" s="7">
         <v>32</v>
       </c>
@@ -1574,7 +1608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="4:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="38" spans="4:9" ht="18" x14ac:dyDescent="0.35">
       <c r="D38" s="7">
         <v>33</v>
       </c>
@@ -1595,7 +1629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="4:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="39" spans="4:9" ht="18" x14ac:dyDescent="0.35">
       <c r="D39" s="7">
         <v>34</v>
       </c>
@@ -1616,7 +1650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="4:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="40" spans="4:9" ht="18" x14ac:dyDescent="0.35">
       <c r="D40" s="7">
         <v>35</v>
       </c>
@@ -1637,7 +1671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="4:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="41" spans="4:9" ht="18" x14ac:dyDescent="0.35">
       <c r="D41" s="7">
         <v>36</v>
       </c>
@@ -1658,7 +1692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="4:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="42" spans="4:9" ht="18" x14ac:dyDescent="0.35">
       <c r="D42" s="7">
         <v>37</v>
       </c>
@@ -1679,7 +1713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="4:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="43" spans="4:9" ht="18" x14ac:dyDescent="0.35">
       <c r="D43" s="7">
         <v>38</v>
       </c>
@@ -1700,7 +1734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="4:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="44" spans="4:9" ht="18" x14ac:dyDescent="0.35">
       <c r="D44" s="7">
         <v>39</v>
       </c>
@@ -1721,7 +1755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="4:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="45" spans="4:9" ht="18" x14ac:dyDescent="0.35">
       <c r="D45" s="7">
         <v>40</v>
       </c>
@@ -1742,14 +1776,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="4:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="46" spans="4:9" ht="18" x14ac:dyDescent="0.35">
       <c r="D46" s="13" t="s">
         <v>20</v>
       </c>
       <c r="E46" s="8"/>
       <c r="F46" s="3">
         <f>SUM(F6:F45)</f>
-        <v>753.6</v>
+        <v>774.18000000000006</v>
       </c>
       <c r="G46" s="4">
         <f t="shared" ref="G46:I46" si="1">SUM(G6:G45)</f>
@@ -1761,7 +1795,7 @@
       </c>
       <c r="I46" s="6">
         <f t="shared" si="1"/>
-        <v>956.42</v>
+        <v>977</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated suzie's excel and xlsx.
</commit_message>
<xml_diff>
--- a/DividendLiberty/Dividend Calculation.xlsx
+++ b/DividendLiberty/Dividend Calculation.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12792" windowHeight="11988"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12792" windowHeight="11988" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Yearly" sheetId="1" r:id="rId1"/>
@@ -581,8 +581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -820,11 +820,11 @@
         <v>0</v>
       </c>
       <c r="F12" s="11">
-        <v>0</v>
+        <v>7.88</v>
       </c>
       <c r="G12" s="12">
         <f t="shared" si="0"/>
-        <v>17.55</v>
+        <v>25.43</v>
       </c>
     </row>
     <row r="13" spans="2:7" ht="18" x14ac:dyDescent="0.35">
@@ -882,11 +882,11 @@
       </c>
       <c r="F15" s="5">
         <f>SUM(F3:F14)</f>
-        <v>129.92000000000002</v>
+        <v>137.80000000000001</v>
       </c>
       <c r="G15" s="6">
         <f>SUM(G3:G14)</f>
-        <v>762.53</v>
+        <v>770.41</v>
       </c>
     </row>
   </sheetData>
@@ -899,8 +899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -971,11 +971,11 @@
         <v>42.16</v>
       </c>
       <c r="H7" s="11">
-        <v>129.91999999999999</v>
+        <v>137.80000000000001</v>
       </c>
       <c r="I7" s="12">
         <f t="shared" ref="I7:I45" si="0">SUM(F7:H7)</f>
-        <v>762.53</v>
+        <v>770.41000000000008</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="18" x14ac:dyDescent="0.35">
@@ -1791,11 +1791,11 @@
       </c>
       <c r="H46" s="5">
         <f t="shared" si="1"/>
-        <v>160.66</v>
+        <v>168.54000000000002</v>
       </c>
       <c r="I46" s="6">
         <f t="shared" si="1"/>
-        <v>977</v>
+        <v>984.88000000000011</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated xlsx and xml.
</commit_message>
<xml_diff>
--- a/DividendLiberty/Dividend Calculation.xlsx
+++ b/DividendLiberty/Dividend Calculation.xlsx
@@ -582,7 +582,7 @@
   <dimension ref="B1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -814,7 +814,7 @@
         <v>14</v>
       </c>
       <c r="D12" s="9">
-        <v>17.55</v>
+        <v>35.24</v>
       </c>
       <c r="E12" s="10">
         <v>0</v>
@@ -824,7 +824,7 @@
       </c>
       <c r="G12" s="12">
         <f t="shared" si="0"/>
-        <v>25.43</v>
+        <v>43.120000000000005</v>
       </c>
     </row>
     <row r="13" spans="2:7" ht="18" x14ac:dyDescent="0.35">
@@ -874,7 +874,7 @@
       </c>
       <c r="D15" s="3">
         <f>SUM(D3:D14)</f>
-        <v>590.44999999999993</v>
+        <v>608.14</v>
       </c>
       <c r="E15" s="4">
         <f>SUM(E3:E14)</f>
@@ -886,7 +886,7 @@
       </c>
       <c r="G15" s="6">
         <f>SUM(G3:G14)</f>
-        <v>770.41</v>
+        <v>788.1</v>
       </c>
     </row>
   </sheetData>
@@ -899,8 +899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="J52" sqref="J52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -965,7 +965,7 @@
         <v>2016</v>
       </c>
       <c r="F7" s="9">
-        <v>590.45000000000005</v>
+        <v>608.14</v>
       </c>
       <c r="G7" s="10">
         <v>42.16</v>
@@ -975,7 +975,7 @@
       </c>
       <c r="I7" s="12">
         <f t="shared" ref="I7:I45" si="0">SUM(F7:H7)</f>
-        <v>770.41000000000008</v>
+        <v>788.09999999999991</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="18" x14ac:dyDescent="0.35">
@@ -1783,7 +1783,7 @@
       <c r="E46" s="8"/>
       <c r="F46" s="3">
         <f>SUM(F6:F45)</f>
-        <v>774.18000000000006</v>
+        <v>791.87</v>
       </c>
       <c r="G46" s="4">
         <f t="shared" ref="G46:I46" si="1">SUM(G6:G45)</f>
@@ -1795,7 +1795,7 @@
       </c>
       <c r="I46" s="6">
         <f t="shared" si="1"/>
-        <v>984.88000000000011</v>
+        <v>1002.5699999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated suzie and total div.
</commit_message>
<xml_diff>
--- a/DividendLiberty/Dividend Calculation.xlsx
+++ b/DividendLiberty/Dividend Calculation.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12792" windowHeight="11988" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12795" windowHeight="11985" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Yearly" sheetId="1" r:id="rId1"/>
     <sheet name="All Time" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -96,7 +96,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -358,23 +358,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -410,23 +393,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -582,25 +548,25 @@
   <dimension ref="B1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B1" s="1">
         <v>2016</v>
       </c>
     </row>
-    <row r="2" spans="2:7" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C2" s="7" t="s">
         <v>0</v>
       </c>
@@ -617,7 +583,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:7" ht="18" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="7">
         <v>1</v>
       </c>
@@ -638,7 +604,7 @@
         <v>30.66</v>
       </c>
     </row>
-    <row r="4" spans="2:7" ht="18" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B4" s="7">
         <v>2</v>
       </c>
@@ -659,7 +625,7 @@
         <v>73.209999999999994</v>
       </c>
     </row>
-    <row r="5" spans="2:7" ht="18" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B5" s="7">
         <v>3</v>
       </c>
@@ -680,7 +646,7 @@
         <v>117.92</v>
       </c>
     </row>
-    <row r="6" spans="2:7" ht="18" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B6" s="7">
         <v>4</v>
       </c>
@@ -701,7 +667,7 @@
         <v>37.21</v>
       </c>
     </row>
-    <row r="7" spans="2:7" ht="18" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B7" s="7">
         <v>5</v>
       </c>
@@ -722,7 +688,7 @@
         <v>70.34</v>
       </c>
     </row>
-    <row r="8" spans="2:7" ht="18" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B8" s="7">
         <v>6</v>
       </c>
@@ -743,7 +709,7 @@
         <v>145.80000000000001</v>
       </c>
     </row>
-    <row r="9" spans="2:7" ht="18" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B9" s="7">
         <v>7</v>
       </c>
@@ -764,7 +730,7 @@
         <v>22.35</v>
       </c>
     </row>
-    <row r="10" spans="2:7" ht="18" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B10" s="7">
         <v>8</v>
       </c>
@@ -785,7 +751,7 @@
         <v>78.61</v>
       </c>
     </row>
-    <row r="11" spans="2:7" ht="18" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B11" s="7">
         <v>9</v>
       </c>
@@ -806,7 +772,7 @@
         <v>168.88</v>
       </c>
     </row>
-    <row r="12" spans="2:7" ht="18" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B12" s="7">
         <v>10</v>
       </c>
@@ -820,14 +786,14 @@
         <v>0</v>
       </c>
       <c r="F12" s="11">
-        <v>7.88</v>
+        <v>13.08</v>
       </c>
       <c r="G12" s="12">
         <f t="shared" si="0"/>
-        <v>43.120000000000005</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" ht="18" x14ac:dyDescent="0.35">
+        <v>48.32</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B13" s="7">
         <v>11</v>
       </c>
@@ -848,7 +814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:7" ht="18" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B14" s="7">
         <v>12</v>
       </c>
@@ -868,7 +834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:7" ht="18" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C15" s="14" t="s">
         <v>20</v>
       </c>
@@ -882,11 +848,11 @@
       </c>
       <c r="F15" s="5">
         <f>SUM(F3:F14)</f>
-        <v>137.80000000000001</v>
+        <v>143.00000000000003</v>
       </c>
       <c r="G15" s="6">
         <f>SUM(G3:G14)</f>
-        <v>788.1</v>
+        <v>793.30000000000007</v>
       </c>
     </row>
   </sheetData>
@@ -899,27 +865,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="J52" sqref="J52"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="E5" s="17" t="s">
         <v>17</v>
       </c>
@@ -936,7 +902,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D6" s="7">
         <v>1</v>
       </c>
@@ -957,7 +923,7 @@
         <v>214.47</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D7" s="7">
         <v>2</v>
       </c>
@@ -965,20 +931,23 @@
         <v>2016</v>
       </c>
       <c r="F7" s="9">
+        <f>Yearly!D15</f>
         <v>608.14</v>
       </c>
       <c r="G7" s="10">
+        <f>Yearly!E15</f>
         <v>42.16</v>
       </c>
       <c r="H7" s="11">
-        <v>137.80000000000001</v>
+        <f>Yearly!F15</f>
+        <v>143.00000000000003</v>
       </c>
       <c r="I7" s="12">
         <f t="shared" ref="I7:I45" si="0">SUM(F7:H7)</f>
-        <v>788.09999999999991</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+        <v>793.3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D8" s="7">
         <v>3</v>
       </c>
@@ -999,7 +968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D9" s="7">
         <v>4</v>
       </c>
@@ -1020,7 +989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D10" s="7">
         <v>5</v>
       </c>
@@ -1041,7 +1010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D11" s="7">
         <v>6</v>
       </c>
@@ -1062,7 +1031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D12" s="7">
         <v>7</v>
       </c>
@@ -1083,7 +1052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D13" s="7">
         <v>8</v>
       </c>
@@ -1104,7 +1073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D14" s="7">
         <v>9</v>
       </c>
@@ -1125,7 +1094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D15" s="7">
         <v>10</v>
       </c>
@@ -1146,7 +1115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D16" s="7">
         <v>11</v>
       </c>
@@ -1167,7 +1136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="4:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="17" spans="4:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D17" s="7">
         <v>12</v>
       </c>
@@ -1188,7 +1157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="4:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="18" spans="4:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D18" s="7">
         <v>13</v>
       </c>
@@ -1209,7 +1178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="4:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="19" spans="4:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D19" s="7">
         <v>14</v>
       </c>
@@ -1230,7 +1199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="4:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="20" spans="4:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D20" s="7">
         <v>15</v>
       </c>
@@ -1251,7 +1220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="4:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="21" spans="4:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D21" s="7">
         <v>16</v>
       </c>
@@ -1272,7 +1241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="4:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="22" spans="4:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D22" s="7">
         <v>17</v>
       </c>
@@ -1293,7 +1262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="4:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="23" spans="4:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D23" s="7">
         <v>18</v>
       </c>
@@ -1314,7 +1283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="4:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="24" spans="4:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D24" s="7">
         <v>19</v>
       </c>
@@ -1335,7 +1304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="4:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="25" spans="4:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D25" s="7">
         <v>20</v>
       </c>
@@ -1356,7 +1325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="4:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="26" spans="4:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D26" s="7">
         <v>21</v>
       </c>
@@ -1377,7 +1346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="4:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="27" spans="4:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D27" s="7">
         <v>22</v>
       </c>
@@ -1398,7 +1367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="4:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="28" spans="4:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D28" s="7">
         <v>23</v>
       </c>
@@ -1419,7 +1388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="4:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="29" spans="4:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D29" s="7">
         <v>24</v>
       </c>
@@ -1440,7 +1409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="4:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="30" spans="4:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D30" s="7">
         <v>25</v>
       </c>
@@ -1461,7 +1430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="4:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="31" spans="4:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D31" s="7">
         <v>26</v>
       </c>
@@ -1482,7 +1451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="4:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="32" spans="4:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D32" s="7">
         <v>27</v>
       </c>
@@ -1503,7 +1472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="4:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="33" spans="4:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D33" s="7">
         <v>28</v>
       </c>
@@ -1524,7 +1493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="4:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="34" spans="4:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D34" s="7">
         <v>29</v>
       </c>
@@ -1545,7 +1514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="4:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="35" spans="4:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D35" s="7">
         <v>30</v>
       </c>
@@ -1566,7 +1535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="4:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="36" spans="4:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D36" s="7">
         <v>31</v>
       </c>
@@ -1587,7 +1556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="4:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="37" spans="4:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D37" s="7">
         <v>32</v>
       </c>
@@ -1608,7 +1577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="4:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="38" spans="4:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D38" s="7">
         <v>33</v>
       </c>
@@ -1629,7 +1598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="4:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="39" spans="4:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D39" s="7">
         <v>34</v>
       </c>
@@ -1650,7 +1619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="4:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="40" spans="4:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D40" s="7">
         <v>35</v>
       </c>
@@ -1671,7 +1640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="4:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="41" spans="4:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D41" s="7">
         <v>36</v>
       </c>
@@ -1692,7 +1661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="4:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="42" spans="4:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D42" s="7">
         <v>37</v>
       </c>
@@ -1713,7 +1682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="4:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="43" spans="4:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D43" s="7">
         <v>38</v>
       </c>
@@ -1734,7 +1703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="4:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="44" spans="4:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D44" s="7">
         <v>39</v>
       </c>
@@ -1755,7 +1724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="4:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="45" spans="4:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D45" s="7">
         <v>40</v>
       </c>
@@ -1776,7 +1745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="4:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="46" spans="4:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D46" s="13" t="s">
         <v>20</v>
       </c>
@@ -1791,11 +1760,11 @@
       </c>
       <c r="H46" s="5">
         <f t="shared" si="1"/>
-        <v>168.54000000000002</v>
+        <v>173.74000000000004</v>
       </c>
       <c r="I46" s="6">
         <f t="shared" si="1"/>
-        <v>1002.5699999999999</v>
+        <v>1007.77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated taxable and year excel.
</commit_message>
<xml_diff>
--- a/DividendLiberty/Dividend Calculation.xlsx
+++ b/DividendLiberty/Dividend Calculation.xlsx
@@ -548,7 +548,7 @@
   <dimension ref="B1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -801,7 +801,7 @@
         <v>15</v>
       </c>
       <c r="D13" s="9">
-        <v>0</v>
+        <v>66.150000000000006</v>
       </c>
       <c r="E13" s="10">
         <v>0</v>
@@ -811,7 +811,7 @@
       </c>
       <c r="G13" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>66.150000000000006</v>
       </c>
     </row>
     <row r="14" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
@@ -840,7 +840,7 @@
       </c>
       <c r="D15" s="3">
         <f>SUM(D3:D14)</f>
-        <v>608.14</v>
+        <v>674.29</v>
       </c>
       <c r="E15" s="4">
         <f>SUM(E3:E14)</f>
@@ -852,7 +852,7 @@
       </c>
       <c r="G15" s="6">
         <f>SUM(G3:G14)</f>
-        <v>793.30000000000007</v>
+        <v>859.45</v>
       </c>
     </row>
   </sheetData>
@@ -865,8 +865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -932,7 +932,7 @@
       </c>
       <c r="F7" s="9">
         <f>Yearly!D15</f>
-        <v>608.14</v>
+        <v>674.29</v>
       </c>
       <c r="G7" s="10">
         <f>Yearly!E15</f>
@@ -944,7 +944,7 @@
       </c>
       <c r="I7" s="12">
         <f t="shared" ref="I7:I45" si="0">SUM(F7:H7)</f>
-        <v>793.3</v>
+        <v>859.44999999999993</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
@@ -1752,7 +1752,7 @@
       <c r="E46" s="8"/>
       <c r="F46" s="3">
         <f>SUM(F6:F45)</f>
-        <v>791.87</v>
+        <v>858.02</v>
       </c>
       <c r="G46" s="4">
         <f t="shared" ref="G46:I46" si="1">SUM(G6:G45)</f>
@@ -1764,7 +1764,7 @@
       </c>
       <c r="I46" s="6">
         <f t="shared" si="1"/>
-        <v>1007.77</v>
+        <v>1073.9199999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated taxable and dividend excel files.
</commit_message>
<xml_diff>
--- a/DividendLiberty/Dividend Calculation.xlsx
+++ b/DividendLiberty/Dividend Calculation.xlsx
@@ -582,7 +582,7 @@
   <dimension ref="B1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="D13:H13"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -835,7 +835,7 @@
         <v>15</v>
       </c>
       <c r="D13" s="9">
-        <v>89.57</v>
+        <v>102.41</v>
       </c>
       <c r="E13" s="10">
         <v>9.1999999999999993</v>
@@ -845,7 +845,7 @@
       </c>
       <c r="G13" s="12">
         <f t="shared" si="0"/>
-        <v>111.72999999999999</v>
+        <v>124.57</v>
       </c>
     </row>
     <row r="14" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
@@ -874,7 +874,7 @@
       </c>
       <c r="D15" s="3">
         <f>SUM(D3:D14)</f>
-        <v>697.71</v>
+        <v>710.55</v>
       </c>
       <c r="E15" s="4">
         <f>SUM(E3:E14)</f>
@@ -886,7 +886,7 @@
       </c>
       <c r="G15" s="6">
         <f>SUM(G3:G14)</f>
-        <v>905.03000000000009</v>
+        <v>917.87000000000012</v>
       </c>
     </row>
   </sheetData>
@@ -899,8 +899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N28" sqref="N28"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -966,7 +966,7 @@
       </c>
       <c r="F7" s="9">
         <f>Yearly!D15</f>
-        <v>697.71</v>
+        <v>710.55</v>
       </c>
       <c r="G7" s="10">
         <f>Yearly!E15</f>
@@ -978,7 +978,7 @@
       </c>
       <c r="I7" s="12">
         <f t="shared" ref="I7:I45" si="0">SUM(F7:H7)</f>
-        <v>905.03000000000009</v>
+        <v>917.87</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
@@ -1786,7 +1786,7 @@
       <c r="E46" s="8"/>
       <c r="F46" s="3">
         <f>SUM(F6:F45)</f>
-        <v>881.44</v>
+        <v>894.28</v>
       </c>
       <c r="G46" s="4">
         <f t="shared" ref="G46:I46" si="1">SUM(G6:G45)</f>
@@ -1798,7 +1798,7 @@
       </c>
       <c r="I46" s="6">
         <f t="shared" si="1"/>
-        <v>1119.5</v>
+        <v>1132.3399999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated taxable and main dividend excel.
</commit_message>
<xml_diff>
--- a/DividendLiberty/Dividend Calculation.xlsx
+++ b/DividendLiberty/Dividend Calculation.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steve Yi\Documents\GitHub\DividendLibertyCommercial\DividendLiberty\bin\Debug\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\OneDrive\Documents\GitHub\DividendLibertyCommercial\DividendLiberty\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Yearly" sheetId="1" r:id="rId1"/>
     <sheet name="All Time" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -96,7 +96,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -358,6 +358,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -393,6 +410,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -548,7 +582,7 @@
   <dimension ref="B1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -822,7 +856,7 @@
         <v>16</v>
       </c>
       <c r="D14" s="9">
-        <v>57.19</v>
+        <v>133.62</v>
       </c>
       <c r="E14" s="10">
         <v>17.100000000000001</v>
@@ -832,7 +866,7 @@
       </c>
       <c r="G14" s="12">
         <f t="shared" si="0"/>
-        <v>93.699999999999989</v>
+        <v>170.13</v>
       </c>
     </row>
     <row r="15" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
@@ -841,7 +875,7 @@
       </c>
       <c r="D15" s="3">
         <f>SUM(D3:D14)</f>
-        <v>767.74</v>
+        <v>844.17</v>
       </c>
       <c r="E15" s="4">
         <f>SUM(E3:E14)</f>
@@ -853,7 +887,7 @@
       </c>
       <c r="G15" s="6">
         <f>SUM(G3:G14)</f>
-        <v>1011.5700000000002</v>
+        <v>1088</v>
       </c>
     </row>
   </sheetData>
@@ -866,8 +900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="M41" sqref="M41"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -933,7 +967,7 @@
       </c>
       <c r="F7" s="9">
         <f>Yearly!D15</f>
-        <v>767.74</v>
+        <v>844.17</v>
       </c>
       <c r="G7" s="10">
         <f>Yearly!E15</f>
@@ -945,7 +979,7 @@
       </c>
       <c r="I7" s="12">
         <f t="shared" ref="I7:I45" si="0">SUM(F7:H7)</f>
-        <v>1011.57</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
@@ -1753,7 +1787,7 @@
       <c r="E46" s="8"/>
       <c r="F46" s="3">
         <f>SUM(F6:F45)</f>
-        <v>951.47</v>
+        <v>1027.8999999999999</v>
       </c>
       <c r="G46" s="4">
         <f t="shared" ref="G46:I46" si="1">SUM(G6:G45)</f>
@@ -1765,7 +1799,7 @@
       </c>
       <c r="I46" s="6">
         <f t="shared" si="1"/>
-        <v>1226.04</v>
+        <v>1302.47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated dividend total and taxable
</commit_message>
<xml_diff>
--- a/DividendLiberty/Dividend Calculation.xlsx
+++ b/DividendLiberty/Dividend Calculation.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\OneDrive\Documents\GitHub\DividendLibertyCommercial\DividendLiberty\bin\Debug\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steve Yi\Documents\GitHub\DividendLibertyCommercial\DividendLiberty\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12795" windowHeight="11985" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12795" windowHeight="11985"/>
   </bookViews>
   <sheets>
     <sheet name="Yearly" sheetId="1" r:id="rId1"/>
     <sheet name="All Time" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="22">
   <si>
     <t>Month</t>
   </si>
@@ -96,7 +96,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -358,23 +358,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -410,23 +393,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -579,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G15"/>
+  <dimension ref="B1:O15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,14 +559,23 @@
     <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B1" s="1">
         <v>2016</v>
       </c>
-    </row>
-    <row r="2" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="J1" s="1">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="2" spans="2:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C2" s="7" t="s">
         <v>0</v>
       </c>
@@ -616,8 +591,23 @@
       <c r="G2" s="15" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="K2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="M2" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="N2" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="O2" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="2:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="7">
         <v>1</v>
       </c>
@@ -637,8 +627,27 @@
         <f>SUM(D3:F3)</f>
         <v>30.66</v>
       </c>
-    </row>
-    <row r="4" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="J3" s="7">
+        <v>1</v>
+      </c>
+      <c r="K3" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="L3" s="9">
+        <v>24.7</v>
+      </c>
+      <c r="M3" s="10">
+        <v>7.55</v>
+      </c>
+      <c r="N3" s="11">
+        <v>0</v>
+      </c>
+      <c r="O3" s="12">
+        <f>SUM(L3:N3)</f>
+        <v>32.25</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B4" s="7">
         <v>2</v>
       </c>
@@ -658,8 +667,27 @@
         <f t="shared" ref="G4:G14" si="0">SUM(D4:F4)</f>
         <v>73.209999999999994</v>
       </c>
-    </row>
-    <row r="5" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="J4" s="7">
+        <v>2</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="L4" s="9">
+        <v>0</v>
+      </c>
+      <c r="M4" s="10">
+        <v>0</v>
+      </c>
+      <c r="N4" s="11">
+        <v>0</v>
+      </c>
+      <c r="O4" s="12">
+        <f t="shared" ref="O4:O14" si="1">SUM(L4:N4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B5" s="7">
         <v>3</v>
       </c>
@@ -679,8 +707,27 @@
         <f t="shared" si="0"/>
         <v>117.92</v>
       </c>
-    </row>
-    <row r="6" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="J5" s="7">
+        <v>3</v>
+      </c>
+      <c r="K5" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="L5" s="9">
+        <v>0</v>
+      </c>
+      <c r="M5" s="10">
+        <v>0</v>
+      </c>
+      <c r="N5" s="11">
+        <v>0</v>
+      </c>
+      <c r="O5" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B6" s="7">
         <v>4</v>
       </c>
@@ -700,8 +747,27 @@
         <f t="shared" si="0"/>
         <v>37.21</v>
       </c>
-    </row>
-    <row r="7" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="J6" s="7">
+        <v>4</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="L6" s="9">
+        <v>0</v>
+      </c>
+      <c r="M6" s="10">
+        <v>0</v>
+      </c>
+      <c r="N6" s="11">
+        <v>0</v>
+      </c>
+      <c r="O6" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B7" s="7">
         <v>5</v>
       </c>
@@ -721,8 +787,27 @@
         <f t="shared" si="0"/>
         <v>70.34</v>
       </c>
-    </row>
-    <row r="8" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="J7" s="7">
+        <v>5</v>
+      </c>
+      <c r="K7" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="L7" s="9">
+        <v>0</v>
+      </c>
+      <c r="M7" s="10">
+        <v>0</v>
+      </c>
+      <c r="N7" s="11">
+        <v>0</v>
+      </c>
+      <c r="O7" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B8" s="7">
         <v>6</v>
       </c>
@@ -742,8 +827,27 @@
         <f t="shared" si="0"/>
         <v>145.80000000000001</v>
       </c>
-    </row>
-    <row r="9" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="J8" s="7">
+        <v>6</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="L8" s="9">
+        <v>0</v>
+      </c>
+      <c r="M8" s="10">
+        <v>0</v>
+      </c>
+      <c r="N8" s="11">
+        <v>0</v>
+      </c>
+      <c r="O8" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B9" s="7">
         <v>7</v>
       </c>
@@ -763,8 +867,27 @@
         <f t="shared" si="0"/>
         <v>22.35</v>
       </c>
-    </row>
-    <row r="10" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="J9" s="7">
+        <v>7</v>
+      </c>
+      <c r="K9" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="L9" s="9">
+        <v>0</v>
+      </c>
+      <c r="M9" s="10">
+        <v>0</v>
+      </c>
+      <c r="N9" s="11">
+        <v>0</v>
+      </c>
+      <c r="O9" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B10" s="7">
         <v>8</v>
       </c>
@@ -784,8 +907,27 @@
         <f t="shared" si="0"/>
         <v>78.61</v>
       </c>
-    </row>
-    <row r="11" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="J10" s="7">
+        <v>8</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="L10" s="9">
+        <v>0</v>
+      </c>
+      <c r="M10" s="10">
+        <v>0</v>
+      </c>
+      <c r="N10" s="11">
+        <v>0</v>
+      </c>
+      <c r="O10" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B11" s="7">
         <v>9</v>
       </c>
@@ -805,8 +947,27 @@
         <f t="shared" si="0"/>
         <v>168.88</v>
       </c>
-    </row>
-    <row r="12" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="J11" s="7">
+        <v>9</v>
+      </c>
+      <c r="K11" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="L11" s="9">
+        <v>0</v>
+      </c>
+      <c r="M11" s="10">
+        <v>0</v>
+      </c>
+      <c r="N11" s="11">
+        <v>0</v>
+      </c>
+      <c r="O11" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B12" s="7">
         <v>10</v>
       </c>
@@ -826,8 +987,27 @@
         <f t="shared" si="0"/>
         <v>48.32</v>
       </c>
-    </row>
-    <row r="13" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="J12" s="7">
+        <v>10</v>
+      </c>
+      <c r="K12" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="L12" s="9">
+        <v>0</v>
+      </c>
+      <c r="M12" s="10">
+        <v>0</v>
+      </c>
+      <c r="N12" s="11">
+        <v>0</v>
+      </c>
+      <c r="O12" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B13" s="7">
         <v>11</v>
       </c>
@@ -847,8 +1027,27 @@
         <f t="shared" si="0"/>
         <v>124.57</v>
       </c>
-    </row>
-    <row r="14" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="J13" s="7">
+        <v>11</v>
+      </c>
+      <c r="K13" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="L13" s="9">
+        <v>0</v>
+      </c>
+      <c r="M13" s="10">
+        <v>0</v>
+      </c>
+      <c r="N13" s="11">
+        <v>0</v>
+      </c>
+      <c r="O13" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B14" s="7">
         <v>12</v>
       </c>
@@ -868,8 +1067,27 @@
         <f t="shared" si="0"/>
         <v>223.13</v>
       </c>
-    </row>
-    <row r="15" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="J14" s="7">
+        <v>12</v>
+      </c>
+      <c r="K14" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="L14" s="9">
+        <v>0</v>
+      </c>
+      <c r="M14" s="10">
+        <v>0</v>
+      </c>
+      <c r="N14" s="11">
+        <v>0</v>
+      </c>
+      <c r="O14" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C15" s="14" t="s">
         <v>20</v>
       </c>
@@ -888,6 +1106,25 @@
       <c r="G15" s="6">
         <f>SUM(G3:G14)</f>
         <v>1141</v>
+      </c>
+      <c r="K15" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="L15" s="3">
+        <f>SUM(L3:L14)</f>
+        <v>24.7</v>
+      </c>
+      <c r="M15" s="4">
+        <f>SUM(M3:M14)</f>
+        <v>7.55</v>
+      </c>
+      <c r="N15" s="5">
+        <f>SUM(N3:N14)</f>
+        <v>0</v>
+      </c>
+      <c r="O15" s="6">
+        <f>SUM(O3:O14)</f>
+        <v>32.25</v>
       </c>
     </row>
   </sheetData>
@@ -900,8 +1137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="L42" sqref="L42"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -990,7 +1227,8 @@
         <v>2017</v>
       </c>
       <c r="F8" s="9">
-        <v>21.64</v>
+        <f>Yearly!L3</f>
+        <v>24.7</v>
       </c>
       <c r="G8" s="10">
         <v>7.55</v>
@@ -1000,7 +1238,7 @@
       </c>
       <c r="I8" s="12">
         <f t="shared" si="0"/>
-        <v>29.19</v>
+        <v>32.25</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
@@ -1787,7 +2025,7 @@
       <c r="E46" s="8"/>
       <c r="F46" s="3">
         <f>SUM(F6:F45)</f>
-        <v>1049.54</v>
+        <v>1052.5999999999999</v>
       </c>
       <c r="G46" s="4">
         <f t="shared" ref="G46:I46" si="1">SUM(G6:G45)</f>
@@ -1799,7 +2037,7 @@
       </c>
       <c r="I46" s="6">
         <f t="shared" si="1"/>
-        <v>1384.66</v>
+        <v>1387.72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated excel for taxable and total dividends.
</commit_message>
<xml_diff>
--- a/DividendLiberty/Dividend Calculation.xlsx
+++ b/DividendLiberty/Dividend Calculation.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\OneDrive\Documents\GitHub\DividendLibertyCommercial\DividendLiberty\bin\Debug\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steve Yi\Documents\GitHub\DividendLibertyCommercial\DividendLiberty\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Yearly" sheetId="1" r:id="rId1"/>
     <sheet name="All Time" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -96,7 +96,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -358,23 +358,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -410,23 +393,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -582,7 +548,7 @@
   <dimension ref="B1:O15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -668,7 +634,7 @@
         <v>5</v>
       </c>
       <c r="L3" s="9">
-        <v>50.57</v>
+        <v>57.62</v>
       </c>
       <c r="M3" s="10">
         <v>12.74</v>
@@ -678,7 +644,7 @@
       </c>
       <c r="O3" s="12">
         <f>SUM(L3:N3)</f>
-        <v>68.570000000000007</v>
+        <v>75.62</v>
       </c>
     </row>
     <row r="4" spans="2:15" ht="18.75" x14ac:dyDescent="0.3">
@@ -1146,7 +1112,7 @@
       </c>
       <c r="L15" s="3">
         <f>SUM(L3:L14)</f>
-        <v>50.57</v>
+        <v>57.62</v>
       </c>
       <c r="M15" s="4">
         <f>SUM(M3:M14)</f>
@@ -1158,7 +1124,7 @@
       </c>
       <c r="O15" s="6">
         <f>SUM(O3:O14)</f>
-        <v>68.570000000000007</v>
+        <v>75.62</v>
       </c>
     </row>
   </sheetData>
@@ -1171,8 +1137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N37" sqref="N37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1262,7 +1228,7 @@
       </c>
       <c r="F8" s="9">
         <f>Yearly!L3</f>
-        <v>50.57</v>
+        <v>57.62</v>
       </c>
       <c r="G8" s="10">
         <v>12.74</v>
@@ -1272,7 +1238,7 @@
       </c>
       <c r="I8" s="12">
         <f t="shared" si="0"/>
-        <v>68.570000000000007</v>
+        <v>75.62</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
@@ -2059,7 +2025,7 @@
       <c r="E46" s="8"/>
       <c r="F46" s="3">
         <f>SUM(F6:F45)</f>
-        <v>1078.4699999999998</v>
+        <v>1085.5199999999998</v>
       </c>
       <c r="G46" s="4">
         <f t="shared" ref="G46:I46" si="1">SUM(G6:G45)</f>
@@ -2071,7 +2037,7 @@
       </c>
       <c r="I46" s="6">
         <f t="shared" si="1"/>
-        <v>1424.04</v>
+        <v>1431.0900000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated xml and excel files for taxable and suzie.
</commit_message>
<xml_diff>
--- a/DividendLiberty/Dividend Calculation.xlsx
+++ b/DividendLiberty/Dividend Calculation.xlsx
@@ -548,7 +548,7 @@
   <dimension ref="B1:O15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,17 +674,17 @@
         <v>6</v>
       </c>
       <c r="L4" s="9">
-        <v>0</v>
+        <v>67.569999999999993</v>
       </c>
       <c r="M4" s="10">
         <v>0</v>
       </c>
       <c r="N4" s="11">
-        <v>0</v>
+        <v>22.05</v>
       </c>
       <c r="O4" s="12">
         <f t="shared" ref="O4:O14" si="1">SUM(L4:N4)</f>
-        <v>0</v>
+        <v>89.61999999999999</v>
       </c>
     </row>
     <row r="5" spans="2:15" ht="18.75" x14ac:dyDescent="0.3">
@@ -1112,7 +1112,7 @@
       </c>
       <c r="L15" s="3">
         <f>SUM(L3:L14)</f>
-        <v>57.62</v>
+        <v>125.19</v>
       </c>
       <c r="M15" s="4">
         <f>SUM(M3:M14)</f>
@@ -1120,11 +1120,11 @@
       </c>
       <c r="N15" s="5">
         <f>SUM(N3:N14)</f>
-        <v>5.26</v>
+        <v>27.310000000000002</v>
       </c>
       <c r="O15" s="6">
         <f>SUM(O3:O14)</f>
-        <v>75.62</v>
+        <v>165.24</v>
       </c>
     </row>
   </sheetData>
@@ -1138,7 +1138,7 @@
   <dimension ref="A1:I46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N37" sqref="N37"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1227,18 +1227,20 @@
         <v>2017</v>
       </c>
       <c r="F8" s="9">
-        <f>Yearly!L3</f>
-        <v>57.62</v>
+        <f>Yearly!L15</f>
+        <v>125.19</v>
       </c>
       <c r="G8" s="10">
+        <f>Yearly!M15</f>
         <v>12.74</v>
       </c>
       <c r="H8" s="11">
-        <v>5.26</v>
+        <f>Yearly!N15</f>
+        <v>27.310000000000002</v>
       </c>
       <c r="I8" s="12">
         <f t="shared" si="0"/>
-        <v>75.62</v>
+        <v>165.24</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
@@ -2025,7 +2027,7 @@
       <c r="E46" s="8"/>
       <c r="F46" s="3">
         <f>SUM(F6:F45)</f>
-        <v>1085.5199999999998</v>
+        <v>1153.0899999999999</v>
       </c>
       <c r="G46" s="4">
         <f t="shared" ref="G46:I46" si="1">SUM(G6:G45)</f>
@@ -2033,11 +2035,11 @@
       </c>
       <c r="H46" s="5">
         <f t="shared" si="1"/>
-        <v>241.18000000000004</v>
+        <v>263.23</v>
       </c>
       <c r="I46" s="6">
         <f t="shared" si="1"/>
-        <v>1431.0900000000001</v>
+        <v>1520.71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated xml and excel taxable and total dividends
</commit_message>
<xml_diff>
--- a/DividendLiberty/Dividend Calculation.xlsx
+++ b/DividendLiberty/Dividend Calculation.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12795" windowHeight="11985"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12795" windowHeight="11985" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Yearly" sheetId="1" r:id="rId1"/>
@@ -547,8 +547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -834,7 +834,7 @@
         <v>10</v>
       </c>
       <c r="L8" s="9">
-        <v>118.95</v>
+        <v>142.19999999999999</v>
       </c>
       <c r="M8" s="10">
         <v>44.98</v>
@@ -844,7 +844,7 @@
       </c>
       <c r="O8" s="12">
         <f t="shared" si="1"/>
-        <v>206.24</v>
+        <v>229.48999999999998</v>
       </c>
     </row>
     <row r="9" spans="2:15" ht="18.75" x14ac:dyDescent="0.3">
@@ -1112,7 +1112,7 @@
       </c>
       <c r="L15" s="3">
         <f>SUM(L3:L14)</f>
-        <v>587.46</v>
+        <v>610.71</v>
       </c>
       <c r="M15" s="4">
         <f>SUM(M3:M14)</f>
@@ -1124,7 +1124,7 @@
       </c>
       <c r="O15" s="6">
         <f>SUM(O3:O14)</f>
-        <v>905.96</v>
+        <v>929.21</v>
       </c>
     </row>
   </sheetData>
@@ -1137,8 +1137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="N29" sqref="N29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1228,7 +1228,7 @@
       </c>
       <c r="F8" s="9">
         <f>Yearly!L15</f>
-        <v>587.46</v>
+        <v>610.71</v>
       </c>
       <c r="G8" s="10">
         <f>Yearly!M15</f>
@@ -1240,7 +1240,7 @@
       </c>
       <c r="I8" s="12">
         <f t="shared" si="0"/>
-        <v>905.96</v>
+        <v>929.21</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
@@ -2027,7 +2027,7 @@
       <c r="E46" s="8"/>
       <c r="F46" s="3">
         <f>SUM(F6:F45)</f>
-        <v>1615.36</v>
+        <v>1638.61</v>
       </c>
       <c r="G46" s="4">
         <f t="shared" ref="G46:I46" si="1">SUM(G6:G45)</f>
@@ -2039,7 +2039,7 @@
       </c>
       <c r="I46" s="6">
         <f t="shared" si="1"/>
-        <v>2261.4300000000003</v>
+        <v>2284.6800000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated roth ira and dividend yearly
</commit_message>
<xml_diff>
--- a/DividendLiberty/Dividend Calculation.xlsx
+++ b/DividendLiberty/Dividend Calculation.xlsx
@@ -565,7 +565,7 @@
   <dimension ref="B1:O37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1097,11 +1097,11 @@
         <v>97.44</v>
       </c>
       <c r="N14" s="7">
-        <v>62.61</v>
+        <v>77.8</v>
       </c>
       <c r="O14" s="8">
         <f t="shared" si="1"/>
-        <v>160.05000000000001</v>
+        <v>175.24</v>
       </c>
     </row>
     <row r="15" spans="2:15" ht="18.75" x14ac:dyDescent="0.3">
@@ -1137,11 +1137,11 @@
       </c>
       <c r="N15" s="16">
         <f>SUM(N3:N14)</f>
-        <v>414.86</v>
+        <v>430.05</v>
       </c>
       <c r="O15" s="17">
         <f>SUM(O3:O14)</f>
-        <v>1460.5900000000001</v>
+        <v>1475.7800000000002</v>
       </c>
     </row>
     <row r="23" spans="2:8" ht="28.5" x14ac:dyDescent="0.45">
@@ -1597,7 +1597,7 @@
       </c>
       <c r="G8" s="7">
         <f>Yearly!N15</f>
-        <v>414.86</v>
+        <v>430.05</v>
       </c>
       <c r="H8" s="18">
         <v>0</v>
@@ -1608,7 +1608,7 @@
       </c>
       <c r="J8" s="8">
         <f t="shared" si="0"/>
-        <v>1460.5900000000001</v>
+        <v>1475.78</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
@@ -2514,7 +2514,7 @@
       </c>
       <c r="G46" s="16">
         <f t="shared" si="1"/>
-        <v>650.78000000000009</v>
+        <v>665.97</v>
       </c>
       <c r="H46" s="19">
         <f>SUM(H6:H45)</f>
@@ -2526,7 +2526,7 @@
       </c>
       <c r="J46" s="17">
         <f t="shared" si="1"/>
-        <v>2832.0900000000006</v>
+        <v>2847.28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>